<commit_message>
Adding to data template some ideas for later additions
</commit_message>
<xml_diff>
--- a/data_files/AllFiles.xlsx
+++ b/data_files/AllFiles.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unordja/PycharmProjects/python-objects-data-standardization/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B6119E-14B5-BD4E-A67E-4B0510C1F685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA15C23-2D27-EB4C-B8A2-BD2B32604858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43900" yWindow="2320" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{6A6B45E4-55B1-D645-8E7B-A71CA400F8DF}"/>
+    <workbookView xWindow="43900" yWindow="2320" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{6A6B45E4-55B1-D645-8E7B-A71CA400F8DF}"/>
   </bookViews>
   <sheets>
     <sheet name="CompanyA" sheetId="1" r:id="rId1"/>
     <sheet name="CompanyB" sheetId="2" r:id="rId2"/>
     <sheet name="CompanyC" sheetId="3" r:id="rId3"/>
     <sheet name="CompanyD" sheetId="4" r:id="rId4"/>
+    <sheet name="Hooli" sheetId="5" r:id="rId5"/>
+    <sheet name="Pied Piper" sheetId="6" r:id="rId6"/>
+    <sheet name="Dunder Mifflin" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
   <si>
     <t>FirstName</t>
   </si>
@@ -258,6 +261,27 @@
   </si>
   <si>
     <t>(656)472-2659</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>CurrentEmployee</t>
+  </si>
+  <si>
+    <t>ManagesOthers</t>
+  </si>
+  <si>
+    <t>HourlyRate</t>
+  </si>
+  <si>
+    <t>CommissionRate</t>
   </si>
 </sst>
 </file>
@@ -309,11 +333,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,7 +655,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +700,7 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2">
@@ -706,7 +729,7 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
       <c r="D3">
@@ -949,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AAEC67-8FF4-7A49-AD1D-06AC5FA117EC}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1043,4 +1066,175 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACB2D32-8627-2E4C-959C-CDE3EC60F289}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA750D69-443F-B144-8C3F-A3EF5EF694AF}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0039C94-B8B4-5D40-B6CC-DEB16EAB7703}">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding more samples of how to work with the data
</commit_message>
<xml_diff>
--- a/data_files/AllFiles.xlsx
+++ b/data_files/AllFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CompanyA" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="160">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -266,6 +266,12 @@
     <t xml:space="preserve">Belson</t>
   </si>
   <si>
+    <t xml:space="preserve">1 Hooli St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palo Alto</t>
+  </si>
+  <si>
     <t xml:space="preserve">CEO</t>
   </si>
   <si>
@@ -278,6 +284,9 @@
     <t xml:space="preserve">Singh</t>
   </si>
   <si>
+    <t xml:space="preserve">7682 Narn Ave</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spiritual Advisor</t>
   </si>
   <si>
@@ -290,6 +299,9 @@
     <t xml:space="preserve">Bighetti</t>
   </si>
   <si>
+    <t xml:space="preserve">987 S Head Ln</t>
+  </si>
+  <si>
     <t xml:space="preserve">Director</t>
   </si>
   <si>
@@ -305,12 +317,21 @@
     <t xml:space="preserve">Hendricks</t>
   </si>
   <si>
+    <t xml:space="preserve"> 5230 Penfield Ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bertram</t>
   </si>
   <si>
     <t xml:space="preserve">Guilfoyle</t>
   </si>
   <si>
+    <t xml:space="preserve">Room 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">CTO</t>
   </si>
   <si>
@@ -320,12 +341,18 @@
     <t xml:space="preserve">Chugtai</t>
   </si>
   <si>
+    <t xml:space="preserve">Room 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jared</t>
   </si>
   <si>
     <t xml:space="preserve">Dunn</t>
   </si>
   <si>
+    <t xml:space="preserve">Garage</t>
+  </si>
+  <si>
     <t xml:space="preserve">COO</t>
   </si>
   <si>
@@ -335,6 +362,9 @@
     <t xml:space="preserve">Hall</t>
   </si>
   <si>
+    <t xml:space="preserve">4475 Mill St</t>
+  </si>
+  <si>
     <t xml:space="preserve">CFO</t>
   </si>
   <si>
@@ -344,6 +374,9 @@
     <t xml:space="preserve">Walton</t>
   </si>
   <si>
+    <t xml:space="preserve">7424 Saw Rd</t>
+  </si>
+  <si>
     <t xml:space="preserve">Developer</t>
   </si>
   <si>
@@ -393,6 +426,87 @@
   </si>
   <si>
     <t xml:space="preserve">9436 S Random LN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zip_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peterson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1834 Cheers Ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norm@pertersonpainting.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mourn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Habitat Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morn@mornshipping.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O’Brien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3951 10 Fwd Avd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Fransico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miles@academy.gov</t>
   </si>
 </sst>
 </file>
@@ -507,7 +621,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -705,10 +819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -803,6 +917,13 @@
         <v>55303</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="kathryn.janeway@voyager.net"/>
@@ -1049,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1100,50 +1221,75 @@
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="0" t="str">
+      <c r="C2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(A2, ".", B3, "@hooli.com")</f>
         <v>Gavin.Singh@hooli.com</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">RANDBETWEEN(2000000000, 9999999999)</f>
-        <v>9563399610</v>
+        <v>5237553443</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>90258</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>50000000</v>
       </c>
-      <c r="M2" s="4" t="b">
+      <c r="M2" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="0" t="str">
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(A3, ".", B4, "@hooli.com")</f>
         <v>Denpok.Bighetti@hooli.com</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">RANDBETWEEN(2000000000, 9999999999)</f>
-        <v>8706914739</v>
+        <v>2467974671</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>150000</v>
@@ -1155,24 +1301,36 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="0" t="e">
-        <f aca="false">_xlfn.CONCAT(A4, ".", #REF!, "@hooli.com")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(A4, ".", B5, "@hooli.com")</f>
+        <v>Nelson.@hooli.com</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <f aca="false">RANDBETWEEN(2000000000, 9999999999)</f>
-        <v>9375180459</v>
+        <v>3378106853</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>90259</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>350000</v>
@@ -1201,8 +1359,8 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1245,18 +1403,41 @@
         <v>76</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A2, ".", B2, "@piper.net")</f>
+        <v>Richard.Hendricks@piper.net</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6506108693</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>350000</v>
@@ -1272,13 +1453,36 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A3, ".", B3, "@piper.net")</f>
+        <v>Bertram.Guilfoyle@piper.net</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6506003214</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>250000</v>
@@ -1294,13 +1498,36 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A4, ".", B4, "@piper.net")</f>
+        <v>Danesh.Chugtai@piper.net</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6504889737</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>96</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>90257</v>
+      </c>
       <c r="J4" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>250000</v>
@@ -1316,13 +1543,36 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A5, ".", B5, "@piper.net")</f>
+        <v>Jared.Dunn@piper.net</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6502304337</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>250000</v>
@@ -1338,13 +1588,33 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A6, ".", B6, "@piper.net")</f>
+        <v>Monica.Hall@piper.net</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6502506598</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>250000</v>
@@ -1360,13 +1630,33 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A7, ".", B7, "@piper.net")</f>
+        <v>Carla.Walton@piper.net</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">RANDBETWEEN(6500000000, 6509999999)</f>
+        <v>6500796051</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>90257</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>150000</v>
@@ -1399,7 +1689,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1447,34 +1737,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2131235468</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>11254</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="L2" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -1483,34 +1773,34 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2134784564</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>11254</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="L3" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -1519,34 +1809,34 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2132145687</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>11254</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="L4" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1574,14 +1864,138 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>12474</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>2152451234</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>21424</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3212478987</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>98471</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>4214754534</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>